<commit_message>
Ajustes para ambientaciones desde CV10
</commit_message>
<xml_diff>
--- a/proyectos/RPA/Ambientacion.xlsx
+++ b/proyectos/RPA/Ambientacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,12 +463,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>v_20230630</t>
+          <t>v_20220331</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SALDOS_DIARIOS_SAP</t>
+          <t>CLIENTES_CNAME</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -478,17 +478,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>6_REFERENCE_DATA</t>
+          <t>1_FACT_DATA_DAILY</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>v_20230331</t>
+          <t>v_20220630</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CUENTAS_CONTABLES_SAP</t>
+          <t>CLIENTES_CNAME</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -503,15 +503,35 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>v_20230630</t>
+          <t>v_20220930</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>GLDMON</t>
+          <t>CLIENTES_CNAME</t>
         </is>
       </c>
       <c r="D4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1_FACT_DATA_DAILY</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>v_20221231</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CLIENTES_CNAME</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>